<commit_message>
add new project for key dataset
</commit_message>
<xml_diff>
--- a/pcor_tools/tests/test_resources/key-datasets-sample-test.xlsx
+++ b/pcor_tools/tests/test_resources/key-datasets-sample-test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pateldes/Documents/github/pcor/pcor_gen3_artifacts/pcor_tools/tests/test_resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36A0A43-CA30-7441-A186-96A3D1616D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74355559-A8BD-A84A-87AD-F30569924D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="25600" activeTab="1" xr2:uid="{637B4EA7-186F-8E46-863B-6788CC042C6C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="23640" activeTab="1" xr2:uid="{637B4EA7-186F-8E46-863B-6788CC042C6C}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="11" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="305">
   <si>
     <t>About this file:</t>
   </si>
@@ -406,18 +406,9 @@
     <t>Grid</t>
   </si>
   <si>
-    <t>NetCDF</t>
-  </si>
-  <si>
     <t>Global</t>
   </si>
   <si>
-    <t>Monthly</t>
-  </si>
-  <si>
-    <t>Geospatial exposure assessment in NIEHS PEGS cohort</t>
-  </si>
-  <si>
     <t>Airports</t>
   </si>
   <si>
@@ -433,21 +424,9 @@
     <t>Roads</t>
   </si>
   <si>
-    <t>R package (amadeus) to download, process, and calculate geographic covariates (https://github.com/kyle-messier/amadeus)</t>
-  </si>
-  <si>
     <t>Environmental Protection Agency (EPA)</t>
   </si>
   <si>
-    <t>Good</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geospatial exposure assessment for public health studies on shorter-term or longer-term outcomes; Geospatial exposure assessment at the individual-level or population-level; Long-term (multi-decade) health cohort studies; Geospatial exposure model development </t>
-  </si>
-  <si>
-    <t>Land Use and Land Cover, Greenness</t>
-  </si>
-  <si>
     <t>Weather and Climate</t>
   </si>
   <si>
@@ -470,60 +449,6 @@
   </si>
   <si>
     <t>Nighttime Light</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modern-Era Retrospective analysis for Research and Applications Version 2 (MERRA-2) </t>
-  </si>
-  <si>
-    <t>0.5 degree x 0.625 degree grid</t>
-  </si>
-  <si>
-    <t>0.5 x 0.625 degree</t>
-  </si>
-  <si>
-    <t>1980 - present</t>
-  </si>
-  <si>
-    <t>Dataset cannot be used to analyze patterns of spatial variability within ~50 km grid resolution grid cells (i.e., within the same city in some cases)</t>
-  </si>
-  <si>
-    <t>M2TMNXLND-071224</t>
-  </si>
-  <si>
-    <t>M2TMNXLND</t>
-  </si>
-  <si>
-    <t>A monthly time-averaged 2-dimensional data collection of land surface parameters is presented in the Modern-Era Retrospective analysis for Research and Applications version 2 (MERRA-2). It provides global model and data assimilation results that incorporate satellite-based observations to predict monthly land surface parameters such as baseflow flux, runoff, surface soil wetness, root zone soil wetness, water at surface layer, water at root zone layer, and soil temperature.</t>
-  </si>
-  <si>
-    <t>US National Aeronautics and Space Administration (NASA) Global Modeling and Assimilation Office (GMAO) Modern-Era Retrospective analysis for Research and Applications Version 2 (MERRA-2) tavgM_2d_lnd_Nx: 2-dimensional, Monthly mean, Time-Averaged, Single-Level, Assimilation, Land Surface Diagnostics (M2TMNXLND), Version 5.12.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Global model and data assimilation incorporating satellite-based observations to predict monthly land surface parameters such as baseflow flux, runoff, surface soil wetness, root zone soil wetness, water at surface layer, water at root zone layer, and soil temperature </t>
-  </si>
-  <si>
-    <t>Land Surface Parameters, Transpiration Energy Flux, Overland Runoff, Soil Moisture, Soil Temperature, Greenness Fraction, Leaf Area Index, Monthly Prediction, Global</t>
-  </si>
-  <si>
-    <t>Transpiration energy flux, greenness fraction, ground heating land, leaf area index, overland runoff</t>
-  </si>
-  <si>
-    <t>Vegetation Greenness, Vegetation Cover, Soil Moisture, Soil Temperature, Runoff</t>
-  </si>
-  <si>
-    <t>https://disc.gsfc.nasa.gov/datasets/M2TMNXLND_5.12.4/summary</t>
-  </si>
-  <si>
-    <t>Global Modeling and Assimilation Office (GMAO) (2015), MERRA-2 tavgM_2d_lnd_Nx: 2d,Monthly mean,Time-Averaged,Single-Level,Assimilation,Land Surface Diagnostics V5.12.4, Greenbelt, MD, USA, Goddard Earth Sciences Data and Information Services Center (GES DISC), [Accessed:  https://doi.org/10.5067/8S35XF81C28F]; Gelaro, R., McCarty, W., Suárez, M. J., Todling, R., Molod, A., Takacs, L., ... &amp; Zhao, B. (2017). The modern-era retrospective analysis for research and applications, version 2 (MERRA-2). Journal of climate, 30(14), 5419-5454.</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.5067/8S35XF81C28F; https://doi.org/10.1175/JCLI-D-16-0758.1</t>
-  </si>
-  <si>
-    <t>Monthly'</t>
-  </si>
-  <si>
-    <t>Land surface parameter estimates for grid cell containing geocoded address</t>
   </si>
   <si>
     <t>Climate Classification</t>
@@ -1074,12 +999,78 @@
   <si>
     <t>Public health emergency/disaster planning and preparedness</t>
   </si>
+  <si>
+    <t>VNP46A2-07</t>
+  </si>
+  <si>
+    <t>VNP46A2</t>
+  </si>
+  <si>
+    <t>NASA- Visible Infrared Imaging Radiometer Suite (VIIRS)</t>
+  </si>
+  <si>
+    <t>Global daily measurements of nocturnal visible and near-infrared light, collected by Day-Night Band sensors in the Visible Infrared Imaging Radiometer Suite (VIIRS), are provided in this dataset at 500 m resolution. The ultra-sensitivity of the VIIRS sensors in lowlight conditions enables the generation of science-quality nighttime products that are suitable for Earth system science and applications due to substantial improvements in sensor resolution and calibration compared to the previous era  products.</t>
+  </si>
+  <si>
+    <t>Redused description by removing some detail about specific NASA satellites, instruments, and former products than may not be needed.</t>
+  </si>
+  <si>
+    <t>US National Aeronautics and Space Administration (NASA) VIIRS/NPP Gap-Filled Lunar BRDF-Adjusted Nighttime Lights Daily L3 Global 500m Linear Lat Lon Grid (VNP46A2)</t>
+  </si>
+  <si>
+    <t>Built Environment, Land Use and Land Cover</t>
+  </si>
+  <si>
+    <t>Daily satellite-based observations of nighttime light with 500 m resolution globally</t>
+  </si>
+  <si>
+    <t>Nocturnal, Nighttime Light, Visible, Near-infrared, Daily Observations, Global</t>
+  </si>
+  <si>
+    <t>Nighttime light</t>
+  </si>
+  <si>
+    <t>HDF</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5067/VIIRS/VNP46A2.001</t>
+  </si>
+  <si>
+    <t>Román, M.O., Wang, Z., Sun, Q., Kalb, V., Miller, S.D., Molthan, A., Schultz, L., Bell, J., Stokes, E.C., Pandey, B. and Seto, K.C., et al. (2018). NASA's Black Marble nighttime lights product suite. Remote Sensing of Environment 210, 113-143. doi:10.1016/j.rse.2018.03.017.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.rse.2018.03.017</t>
+  </si>
+  <si>
+    <t>500 m</t>
+  </si>
+  <si>
+    <t>2012 - present</t>
+  </si>
+  <si>
+    <t>Daily</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geospatial exposure model development </t>
+  </si>
+  <si>
+    <t>Nighttime light brightness for grid cell containing geocoded address</t>
+  </si>
+  <si>
+    <t>Dataset includes data quality information</t>
+  </si>
+  <si>
+    <t>Data quality varies due to differences in cloud cover, moonlight, and air quality by time and location</t>
+  </si>
+  <si>
+    <t>NASA Black Marble Tools for access and analysis of nighttime light data, including R package and Python library (https://blackmarble.gsfc.nasa.gov/Tools.html)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1163,18 +1154,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -1239,13 +1218,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF00B050"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF444444"/>
       <name val="Arial"/>
@@ -1264,6 +1236,12 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1536,7 +1514,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1600,23 +1578,14 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1631,28 +1600,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1698,10 +1667,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1713,18 +1679,15 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1772,6 +1735,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1796,10 +1768,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2113,67 +2081,67 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="83"/>
+      <c r="B2" s="78"/>
     </row>
     <row r="3" spans="1:6" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="84"/>
+      <c r="B3" s="79"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="83" t="s">
+      <c r="A5" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="83"/>
+      <c r="B5" s="78"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="78"/>
+      <c r="B6" s="73"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="78"/>
+      <c r="B7" s="73"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="78"/>
+      <c r="B8" s="73"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="77" t="s">
+      <c r="A9" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="78"/>
+      <c r="B9" s="73"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="77" t="s">
+      <c r="A10" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="78"/>
+      <c r="B10" s="73"/>
     </row>
     <row r="11" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="79" t="s">
+      <c r="A11" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="80"/>
+      <c r="B11" s="75"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="82"/>
+      <c r="B13" s="77"/>
       <c r="C13" s="26" t="s">
         <v>10</v>
       </c>
@@ -2501,362 +2469,362 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="72"/>
-    <col min="2" max="2" width="26" style="37" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" style="37" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" style="37" customWidth="1"/>
-    <col min="5" max="6" width="24.6640625" style="37" customWidth="1"/>
-    <col min="7" max="8" width="33.5" style="37" customWidth="1"/>
-    <col min="9" max="9" width="31" style="37" customWidth="1"/>
-    <col min="10" max="10" width="21.1640625" style="37" customWidth="1"/>
-    <col min="11" max="11" width="14.83203125" style="37" customWidth="1"/>
-    <col min="12" max="12" width="28.83203125" style="37" customWidth="1"/>
-    <col min="13" max="13" width="28.5" style="37" customWidth="1"/>
-    <col min="14" max="14" width="26.1640625" style="37" customWidth="1"/>
-    <col min="15" max="15" width="26.1640625" style="66" customWidth="1"/>
-    <col min="16" max="16" width="13.33203125" style="37" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="67"/>
+    <col min="2" max="2" width="26" style="34" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="34" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" style="34" customWidth="1"/>
+    <col min="5" max="6" width="24.6640625" style="34" customWidth="1"/>
+    <col min="7" max="8" width="33.5" style="34" customWidth="1"/>
+    <col min="9" max="9" width="31" style="34" customWidth="1"/>
+    <col min="10" max="10" width="21.1640625" style="34" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" style="34" customWidth="1"/>
+    <col min="12" max="12" width="28.83203125" style="34" customWidth="1"/>
+    <col min="13" max="13" width="28.5" style="34" customWidth="1"/>
+    <col min="14" max="14" width="26.1640625" style="34" customWidth="1"/>
+    <col min="15" max="15" width="26.1640625" style="62" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" style="34" customWidth="1"/>
     <col min="17" max="17" width="19.83203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="32.1640625" style="67" customWidth="1"/>
+    <col min="18" max="18" width="32.1640625" style="63" customWidth="1"/>
     <col min="19" max="19" width="38.83203125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="16.6640625" style="37" customWidth="1"/>
-    <col min="21" max="21" width="14.1640625" style="66" customWidth="1"/>
-    <col min="22" max="22" width="12.6640625" style="37" customWidth="1"/>
-    <col min="23" max="24" width="12.6640625" style="66" customWidth="1"/>
-    <col min="25" max="25" width="12.33203125" style="37" customWidth="1"/>
-    <col min="26" max="26" width="12.5" style="37" customWidth="1"/>
-    <col min="27" max="31" width="12.5" style="66" customWidth="1"/>
-    <col min="32" max="32" width="12.5" style="68" customWidth="1"/>
-    <col min="33" max="34" width="22.6640625" style="37" customWidth="1"/>
-    <col min="35" max="35" width="28.83203125" style="37" customWidth="1"/>
-    <col min="36" max="36" width="29.83203125" style="37" customWidth="1"/>
-    <col min="37" max="37" width="20.5" style="37" customWidth="1"/>
-    <col min="38" max="38" width="30.33203125" style="67" customWidth="1"/>
-    <col min="39" max="16384" width="10.83203125" style="37"/>
+    <col min="20" max="20" width="16.6640625" style="34" customWidth="1"/>
+    <col min="21" max="21" width="14.1640625" style="62" customWidth="1"/>
+    <col min="22" max="22" width="12.6640625" style="34" customWidth="1"/>
+    <col min="23" max="24" width="12.6640625" style="62" customWidth="1"/>
+    <col min="25" max="25" width="12.33203125" style="34" customWidth="1"/>
+    <col min="26" max="26" width="12.5" style="34" customWidth="1"/>
+    <col min="27" max="31" width="12.5" style="62" customWidth="1"/>
+    <col min="32" max="32" width="12.5" style="64" customWidth="1"/>
+    <col min="33" max="34" width="22.6640625" style="34" customWidth="1"/>
+    <col min="35" max="35" width="28.83203125" style="34" customWidth="1"/>
+    <col min="36" max="36" width="29.83203125" style="34" customWidth="1"/>
+    <col min="37" max="37" width="20.5" style="34" customWidth="1"/>
+    <col min="38" max="38" width="30.33203125" style="63" customWidth="1"/>
+    <col min="39" max="16384" width="10.83203125" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J1" s="85" t="s">
+      <c r="J1" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="85"/>
-      <c r="O1" s="85"/>
-      <c r="P1" s="85"/>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="86"/>
-      <c r="S1" s="75"/>
-      <c r="T1" s="87" t="s">
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="80"/>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="81"/>
+      <c r="S1" s="70"/>
+      <c r="T1" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="U1" s="88"/>
-      <c r="V1" s="88"/>
-      <c r="W1" s="88"/>
-      <c r="X1" s="88"/>
-      <c r="Y1" s="88"/>
-      <c r="Z1" s="88"/>
-      <c r="AA1" s="88"/>
-      <c r="AB1" s="88"/>
-      <c r="AC1" s="88"/>
-      <c r="AD1" s="88"/>
-      <c r="AE1" s="88"/>
-      <c r="AF1" s="89"/>
-      <c r="AG1" s="90" t="s">
+      <c r="U1" s="83"/>
+      <c r="V1" s="83"/>
+      <c r="W1" s="83"/>
+      <c r="X1" s="83"/>
+      <c r="Y1" s="83"/>
+      <c r="Z1" s="83"/>
+      <c r="AA1" s="83"/>
+      <c r="AB1" s="83"/>
+      <c r="AC1" s="83"/>
+      <c r="AD1" s="83"/>
+      <c r="AE1" s="83"/>
+      <c r="AF1" s="84"/>
+      <c r="AG1" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="AH1" s="90"/>
-      <c r="AI1" s="90"/>
-      <c r="AJ1" s="90"/>
-      <c r="AK1" s="90"/>
-      <c r="AL1" s="90"/>
-      <c r="AM1" s="50" t="s">
+      <c r="AH1" s="85"/>
+      <c r="AI1" s="85"/>
+      <c r="AJ1" s="85"/>
+      <c r="AK1" s="85"/>
+      <c r="AL1" s="85"/>
+      <c r="AM1" s="47" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:39" s="60" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A2" s="73" t="s">
+    <row r="2" spans="1:39" s="57" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="51" t="s">
+      <c r="H2" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="I2" s="69" t="s">
+      <c r="I2" s="65" t="s">
         <v>76</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="35" t="s">
+      <c r="K2" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="L2" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="N2" s="35" t="s">
+      <c r="N2" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="O2" s="52"/>
-      <c r="P2" s="35" t="s">
+      <c r="O2" s="49"/>
+      <c r="P2" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="Q2" s="35" t="s">
+      <c r="Q2" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="R2" s="53" t="s">
+      <c r="R2" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="S2" s="35" t="s">
+      <c r="S2" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="T2" s="54" t="s">
+      <c r="T2" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="U2" s="52"/>
-      <c r="V2" s="54" t="s">
+      <c r="U2" s="49"/>
+      <c r="V2" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="W2" s="55"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="54" t="s">
+      <c r="W2" s="52"/>
+      <c r="X2" s="52"/>
+      <c r="Y2" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="Z2" s="54" t="s">
+      <c r="Z2" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="AA2" s="55"/>
-      <c r="AB2" s="55"/>
-      <c r="AC2" s="55"/>
-      <c r="AD2" s="55"/>
-      <c r="AE2" s="55"/>
-      <c r="AF2" s="56"/>
-      <c r="AG2" s="57" t="s">
+      <c r="AA2" s="52"/>
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="52"/>
+      <c r="AD2" s="52"/>
+      <c r="AE2" s="52"/>
+      <c r="AF2" s="53"/>
+      <c r="AG2" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="AH2" s="57" t="s">
+      <c r="AH2" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="AI2" s="57" t="s">
+      <c r="AI2" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="AJ2" s="57" t="s">
+      <c r="AJ2" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="AK2" s="57" t="s">
+      <c r="AK2" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="AL2" s="58" t="s">
+      <c r="AL2" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="AM2" s="59" t="s">
+      <c r="AM2" s="56" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:39" s="60" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="74"/>
-      <c r="B3" s="62" t="s">
+    <row r="3" spans="1:39" s="57" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="69"/>
+      <c r="B3" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="36" t="s">
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="60" t="s">
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="N3" s="36"/>
-      <c r="O3" s="55" t="s">
+      <c r="N3" s="33"/>
+      <c r="O3" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="P3" s="36" t="s">
+      <c r="P3" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="Q3" s="36" t="s">
+      <c r="Q3" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="R3" s="63" t="s">
+      <c r="R3" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="S3" s="36"/>
-      <c r="T3" s="36" t="s">
+      <c r="S3" s="33"/>
+      <c r="T3" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="U3" s="55" t="s">
+      <c r="U3" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="V3" s="36"/>
-      <c r="W3" s="55" t="s">
+      <c r="V3" s="33"/>
+      <c r="W3" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="X3" s="55" t="s">
+      <c r="X3" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="Y3" s="36"/>
-      <c r="Z3" s="36"/>
-      <c r="AA3" s="55" t="s">
+      <c r="Y3" s="33"/>
+      <c r="Z3" s="33"/>
+      <c r="AA3" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="AB3" s="55" t="s">
+      <c r="AB3" s="52" t="s">
         <v>105</v>
       </c>
-      <c r="AC3" s="55" t="s">
+      <c r="AC3" s="52" t="s">
         <v>106</v>
       </c>
-      <c r="AD3" s="55" t="s">
+      <c r="AD3" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="AE3" s="55" t="s">
+      <c r="AE3" s="52" t="s">
         <v>108</v>
       </c>
-      <c r="AF3" s="56" t="s">
+      <c r="AF3" s="53" t="s">
         <v>109</v>
       </c>
-      <c r="AG3" s="36"/>
-      <c r="AH3" s="36"/>
-      <c r="AI3" s="36"/>
-      <c r="AJ3" s="36"/>
-      <c r="AK3" s="36"/>
-      <c r="AL3" s="63"/>
-      <c r="AM3" s="64"/>
-    </row>
-    <row r="4" spans="1:39" s="1" customFormat="1" ht="345" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="72" t="s">
+      <c r="AG3" s="33"/>
+      <c r="AH3" s="33"/>
+      <c r="AI3" s="33"/>
+      <c r="AJ3" s="33"/>
+      <c r="AK3" s="33"/>
+      <c r="AL3" s="60"/>
+      <c r="AM3" s="61"/>
+    </row>
+    <row r="4" spans="1:39" s="1" customFormat="1" ht="351.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="67" t="s">
         <v>110</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>140</v>
+        <v>283</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>141</v>
+        <v>284</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>135</v>
+        <v>285</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="F4" s="29"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="I4" s="70" t="s">
-        <v>124</v>
+        <v>125</v>
+      </c>
+      <c r="F4" s="86"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27" t="s">
+        <v>286</v>
+      </c>
+      <c r="I4" s="87" t="s">
+        <v>287</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>143</v>
+        <v>288</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>126</v>
+        <v>289</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="M4" s="27" t="s">
-        <v>145</v>
+        <v>290</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>291</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>146</v>
+        <v>292</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="P4" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q4" s="88" t="s">
+        <v>294</v>
+      </c>
+      <c r="R4" s="31" t="s">
+        <v>295</v>
+      </c>
+      <c r="S4" s="27" t="s">
+        <v>296</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="Q4" s="65" t="s">
-        <v>148</v>
-      </c>
-      <c r="R4" s="34" t="s">
-        <v>149</v>
-      </c>
-      <c r="S4" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="U4" s="8" t="s">
         <v>112</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="W4" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="W4" s="8" t="s">
         <v>112</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>137</v>
+        <v>297</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>138</v>
+        <v>298</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>115</v>
+        <v>299</v>
       </c>
       <c r="AA4" s="8">
-        <v>1980</v>
+        <v>2012</v>
       </c>
       <c r="AB4" s="8">
         <v>2024</v>
       </c>
       <c r="AC4" s="8"/>
       <c r="AD4" s="8" t="s">
-        <v>151</v>
+        <v>299</v>
       </c>
       <c r="AE4" s="8"/>
       <c r="AF4" s="10"/>
       <c r="AG4" s="7" t="s">
-        <v>125</v>
+        <v>300</v>
       </c>
       <c r="AH4" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="AI4" s="7"/>
+        <v>301</v>
+      </c>
+      <c r="AI4" s="7" t="s">
+        <v>302</v>
+      </c>
       <c r="AJ4" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="AK4" s="7" t="s">
-        <v>116</v>
-      </c>
+        <v>303</v>
+      </c>
+      <c r="AK4" s="7"/>
       <c r="AL4" s="6" t="s">
-        <v>122</v>
+        <v>304</v>
       </c>
       <c r="AM4" s="4">
-        <v>45370</v>
+        <v>45334</v>
       </c>
     </row>
   </sheetData>
@@ -2867,7 +2835,7 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="Q4" r:id="rId1" xr:uid="{E97DAC12-9951-C64C-81BB-B9F3ECB4BE06}"/>
+    <hyperlink ref="Q4" r:id="rId1" xr:uid="{8A0E72C0-B9A1-954A-A510-C3FDC600E9AA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="171" orientation="landscape" r:id="rId2"/>
@@ -2889,55 +2857,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>163</v>
+      <c r="A1" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="31"/>
+      <c r="A2" s="28"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="B15" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2967,608 +2935,608 @@
   <sheetData>
     <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="12" customFormat="1" ht="20" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>111</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>111</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>111</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="12" customFormat="1" ht="20" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>111</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="12" customFormat="1" ht="20" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>111</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="12" customFormat="1" ht="20" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>111</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>194</v>
+        <v>169</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>111</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>195</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>196</v>
+        <v>171</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>198</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>199</v>
+        <v>174</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>202</v>
+        <v>177</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>203</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>208</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>211</v>
-      </c>
       <c r="C18" s="15" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>212</v>
+        <v>187</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>213</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>214</v>
+        <v>189</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>215</v>
+        <v>190</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>216</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>217</v>
+        <v>192</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>219</v>
+        <v>194</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>220</v>
+        <v>195</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>220</v>
+        <v>195</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>221</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>226</v>
+        <v>201</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>228</v>
+        <v>203</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>233</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B29" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="C29" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="F29" s="15" t="s">
         <v>211</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>237</v>
+        <v>212</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>239</v>
+        <v>214</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>241</v>
+        <v>216</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>242</v>
+        <v>217</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>243</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>241</v>
+        <v>216</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>242</v>
+        <v>217</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>245</v>
+        <v>220</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>246</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -3586,277 +3554,277 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="48" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.1640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" style="45" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.1640625" style="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="37" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="39" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B19" s="38" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B20" s="38" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B22" s="38" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="41" t="s">
+        <v>226</v>
+      </c>
+      <c r="B23" s="38" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B24" s="38" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="40" t="s">
+        <v>243</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="42" t="s">
+        <v>245</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="43" t="s">
         <v>247</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B27" s="38" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="44" t="s">
         <v>249</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B28" s="38" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="39" t="s">
+        <v>226</v>
+      </c>
+      <c r="B29" s="38" t="s">
         <v>251</v>
       </c>
-      <c r="B3" s="41" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B4" s="41" t="s">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B30" s="38" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B5" s="41" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B6" s="41" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B7" s="41" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B8" s="41" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B31" s="38" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B9" s="41" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B32" s="38" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B12" s="41" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B33" s="38" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B13" s="41" t="s">
+    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="B34" s="46" t="s">
         <v>256</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B14" s="41" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B15" s="41" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B16" s="41" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B17" s="41" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B18" s="41" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B19" s="41" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B20" s="41" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B21" s="41" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B22" s="41" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="44" t="s">
-        <v>251</v>
-      </c>
-      <c r="B23" s="41" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B24" s="41" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="43" t="s">
-        <v>268</v>
-      </c>
-      <c r="B25" s="41" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="45" t="s">
-        <v>270</v>
-      </c>
-      <c r="B26" s="41" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="46" t="s">
-        <v>272</v>
-      </c>
-      <c r="B27" s="41" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="47" t="s">
-        <v>274</v>
-      </c>
-      <c r="B28" s="41" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="42" t="s">
-        <v>251</v>
-      </c>
-      <c r="B29" s="41" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B30" s="41" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B31" s="41" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B32" s="41" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B33" s="41" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="B34" s="49" t="s">
-        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -3879,115 +3847,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="66" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="71" t="s">
+        <v>259</v>
+      </c>
+      <c r="B2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="71" t="s">
+        <v>261</v>
+      </c>
+      <c r="B3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="71" t="s">
+        <v>263</v>
+      </c>
+      <c r="B4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="71" t="s">
+        <v>265</v>
+      </c>
+      <c r="B5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="71" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="71" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="B8" s="71" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="71" t="s">
+        <v>271</v>
+      </c>
+      <c r="B9" s="71"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="71" t="s">
+        <v>272</v>
+      </c>
+      <c r="B10" s="71"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="71" t="s">
+        <v>273</v>
+      </c>
+      <c r="B11" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="71" t="s">
+        <v>275</v>
+      </c>
+      <c r="B12" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="71" t="s">
+        <v>277</v>
+      </c>
+      <c r="B13" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="71" t="s">
+        <v>279</v>
+      </c>
+      <c r="B14" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="71" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="71" t="s">
         <v>282</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="76" t="s">
-        <v>284</v>
-      </c>
-      <c r="B2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="76" t="s">
-        <v>286</v>
-      </c>
-      <c r="B3" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="76" t="s">
-        <v>288</v>
-      </c>
-      <c r="B4" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="76" t="s">
-        <v>290</v>
-      </c>
-      <c r="B5" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="76" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="76" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="76" t="s">
-        <v>294</v>
-      </c>
-      <c r="B8" s="76" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="76" t="s">
-        <v>296</v>
-      </c>
-      <c r="B9" s="76"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="76" t="s">
-        <v>297</v>
-      </c>
-      <c r="B10" s="76"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="76" t="s">
-        <v>298</v>
-      </c>
-      <c r="B11" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="76" t="s">
-        <v>300</v>
-      </c>
-      <c r="B12" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="76" t="s">
-        <v>302</v>
-      </c>
-      <c r="B13" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="76" t="s">
-        <v>304</v>
-      </c>
-      <c r="B14" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="76" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="76" t="s">
-        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -4005,17 +3973,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2de882ca-9509-47c1-8c64-fb583c88719d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="687fcabb-7907-411d-9d68-e27ef4ca3abf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BAD4B8DE911AC343BFDC9276B63D4692" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="da715119a34c6f135312c33e82e796ae">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2de882ca-9509-47c1-8c64-fb583c88719d" xmlns:ns3="687fcabb-7907-411d-9d68-e27ef4ca3abf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="302baa9287f9ef7b911acf2a14e6f5ac" ns2:_="" ns3:_="">
     <xsd:import namespace="2de882ca-9509-47c1-8c64-fb583c88719d"/>
@@ -4244,6 +4201,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2de882ca-9509-47c1-8c64-fb583c88719d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="687fcabb-7907-411d-9d68-e27ef4ca3abf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47660805-3115-4497-A410-CE66A09F4931}">
   <ds:schemaRefs>
@@ -4253,17 +4221,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52A191B0-C3D7-488C-ACAC-B7E55D563B0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2de882ca-9509-47c1-8c64-fb583c88719d"/>
-    <ds:schemaRef ds:uri="687fcabb-7907-411d-9d68-e27ef4ca3abf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F99A077B-1777-4449-B703-6FEE4C1C2ECC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4282,6 +4239,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52A191B0-C3D7-488C-ACAC-B7E55D563B0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2de882ca-9509-47c1-8c64-fb583c88719d"/>
+    <ds:schemaRef ds:uri="687fcabb-7907-411d-9d68-e27ef4ca3abf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{14b77578-9773-42d5-8507-251ca2dc2b06}" enabled="0" method="" siteId="{14b77578-9773-42d5-8507-251ca2dc2b06}" removed="1"/>

</xml_diff>